<commit_message>
Added code for WFMTimeCardExceptions TestCase
</commit_message>
<xml_diff>
--- a/Data/Timecard_Total_Amy.xlsx
+++ b/Data/Timecard_Total_Amy.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B9EC8B-500C-469E-B470-236DFBC8C102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Tabelle1" state="visible" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>EmpID</t>
   </si>
@@ -68,45 +70,105 @@
   </si>
   <si>
     <t>SK-Tracking Quaterly Hours</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Estimated Date</t>
+  </si>
+  <si>
+    <t>Revised Date (if needed)</t>
+  </si>
+  <si>
+    <t>Timecard Exceptions</t>
+  </si>
+  <si>
+    <t>Madhukar</t>
+  </si>
+  <si>
+    <t>13th Dec'24</t>
+  </si>
+  <si>
+    <t>6th Jan'24</t>
+  </si>
+  <si>
+    <t>Timecard Premiums</t>
+  </si>
+  <si>
+    <t>Gayatri</t>
+  </si>
+  <si>
+    <t>Overtime Approval</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
       <family val="3"/>
-      <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <name val="Consolas"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9C9C9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -114,11 +176,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -126,6 +227,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -134,14 +244,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -420,22 +530,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="140" zoomScaleNormal="140">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10649095</v>
       </c>
@@ -463,7 +573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10649095</v>
       </c>
@@ -477,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>10649095</v>
       </c>
@@ -491,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>10649095</v>
       </c>
@@ -505,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10649095</v>
       </c>
@@ -519,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10649095</v>
       </c>
@@ -533,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>10649095</v>
       </c>
@@ -547,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>10649095</v>
       </c>
@@ -561,19 +671,110 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="15.6" customHeight="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"""Failed"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2078ECA6-37EE-4EC9-9A0B-DD240B836FA9}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>